<commit_message>
-Test (Developer) mode added. -Maximum result page limit set to 500.
</commit_message>
<xml_diff>
--- a/parametreler.xlsx
+++ b/parametreler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ferhat\Documents\UiPath\Sahibinden_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAADF06-9F93-4D51-BFCF-B39D88518F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D71CD36-7296-40F8-AE95-9855C4ADD345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{19E220D8-1938-42AA-9C5B-C80B7A6E309D}"/>
   </bookViews>
@@ -452,7 +452,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>